<commit_message>
build integrator and builder for SemesterGradesSheet
</commit_message>
<xml_diff>
--- a/AppData/Reports/SemesterGradesSheet/Template.xlsx
+++ b/AppData/Reports/SemesterGradesSheet/Template.xlsx
@@ -55,9 +55,6 @@
     <t>7 (семь)</t>
   </si>
   <si>
-    <t>ГЛАВНОЕ УПРАВЛЕНИЕ ПО ОБРАЗОВАНИЮ БРЕСТСКОГО ОБЛИСПОЛКОМА</t>
-  </si>
-  <si>
     <t>УО «Пинский государственный профессионально-технический колледж легкой промышленности»</t>
   </si>
   <si>
@@ -230,13 +227,60 @@
   </si>
   <si>
     <t>(подпись)</t>
+  </si>
+  <si>
+    <r>
+      <t>ГЛАВНОЕ УП</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>РАВЛЕНИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Е ПО ОБРАЗОВАН</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>ИЮ БРЕСТСКО</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>ГО ОБЛИСПОЛКОМА</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +347,14 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -345,44 +397,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,176 +735,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="14"/>
+      <c r="E9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>1</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>5.6</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>7</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="15" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A7:G7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add template parametrizing methods, develop ReportIntegrator
</commit_message>
<xml_diff>
--- a/AppData/Reports/SemesterGradesSheet/Template.xlsx
+++ b/AppData/Reports/SemesterGradesSheet/Template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>№ п/п</t>
   </si>
@@ -46,15 +46,6 @@
 учащегося</t>
   </si>
   <si>
-    <t>Корневич Максим Александрович</t>
-  </si>
-  <si>
-    <t>зачтено</t>
-  </si>
-  <si>
-    <t>7 (семь)</t>
-  </si>
-  <si>
     <t>УО «Пинский государственный профессионально-технический колледж легкой промышленности»</t>
   </si>
   <si>
@@ -274,6 +265,24 @@
       </rPr>
       <t>ГО ОБЛИСПОЛКОМА</t>
     </r>
+  </si>
+  <si>
+    <t>{StudentIndex}</t>
+  </si>
+  <si>
+    <t>{StudentName}</t>
+  </si>
+  <si>
+    <t>{OKRAvg}</t>
+  </si>
+  <si>
+    <t>{LPR}</t>
+  </si>
+  <si>
+    <t>{CourseGrade}</t>
+  </si>
+  <si>
+    <t>{SemesterGrade}</t>
   </si>
 </sst>
 </file>
@@ -719,12 +728,12 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
@@ -736,7 +745,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -747,7 +756,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -759,7 +768,7 @@
     <row r="3" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -770,7 +779,7 @@
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -790,7 +799,7 @@
     </row>
     <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -835,52 +844,52 @@
       <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>1</v>
+      <c r="A11" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3">
-        <v>5.6</v>
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="3">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>

</xml_diff>

<commit_message>
refactoring base report components, finalize SemesterGradesSheet
</commit_message>
<xml_diff>
--- a/AppData/Reports/SemesterGradesSheet/Template.xlsx
+++ b/AppData/Reports/SemesterGradesSheet/Template.xlsx
@@ -354,44 +354,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,7 +676,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,175 +692,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A7:G7"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add ParentOrganisationName and OrganisationName params, improve project model
</commit_message>
<xml_diff>
--- a/AppData/Reports/SemesterGradesSheet/Template.xlsx
+++ b/AppData/Reports/SemesterGradesSheet/Template.xlsx
@@ -46,12 +46,6 @@
 учащегося</t>
   </si>
   <si>
-    <t>ГЛАВНОЕ УПРАВЛЕНИЕ ПО ОБРАЗОВАНИЮ БРЕСТСКОГО ОБЛИСПОЛКОМА</t>
-  </si>
-  <si>
-    <t>УО «Пинский государственный профессионально-технический колледж легкой промышленности»</t>
-  </si>
-  <si>
     <t>ВЕДОМОСТЬ</t>
   </si>
   <si>
@@ -239,6 +233,12 @@
   </si>
   <si>
     <t xml:space="preserve">   {SemesterGrade}</t>
+  </si>
+  <si>
+    <t>{ParentOrganizationName}</t>
+  </si>
+  <si>
+    <t>{OrganizationName}</t>
   </si>
 </sst>
 </file>
@@ -357,40 +357,40 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -676,7 +676,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,49 +692,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="A1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="A2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="A4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -746,121 +746,121 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="A7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="15"/>
+      <c r="E9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="D11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="E11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="15"/>
+      <c r="F11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12" t="s">
+      <c r="A12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A7:G7"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:G13"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
refactor SemesterGradesSheet and move reports to "reports" napespace
</commit_message>
<xml_diff>
--- a/AppData/Reports/SemesterGradesSheet/Template.xlsx
+++ b/AppData/Reports/SemesterGradesSheet/Template.xlsx
@@ -232,13 +232,13 @@
     <t xml:space="preserve"> {CuratorName} </t>
   </si>
   <si>
-    <t xml:space="preserve">   {SemesterGrade}</t>
-  </si>
-  <si>
     <t>{ParentOrganizationName}</t>
   </si>
   <si>
     <t>{OrganizationName}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   {SemesterGrade} ({SemesterGradeText})</t>
   </si>
 </sst>
 </file>
@@ -363,35 +363,35 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,7 +676,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,49 +692,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -758,38 +758,38 @@
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="14" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -808,59 +808,59 @@
         <v>17</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A7:G7"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
SemesterGradesSheet finalize validator, add GradeValue.ToString , implove GradeQuery
</commit_message>
<xml_diff>
--- a/AppData/Reports/SemesterGradesSheet/Template.xlsx
+++ b/AppData/Reports/SemesterGradesSheet/Template.xlsx
@@ -67,9 +67,6 @@
     <t>{StudentName}</t>
   </si>
   <si>
-    <t>{OKRAvg}</t>
-  </si>
-  <si>
     <t>{LPR}</t>
   </si>
   <si>
@@ -238,7 +235,10 @@
     <t>{OrganizationName}</t>
   </si>
   <si>
-    <t xml:space="preserve">   {SemesterGrade} ({SemesterGradeText})</t>
+    <t>{OKRs}</t>
+  </si>
+  <si>
+    <t>{SemesterGrade}</t>
   </si>
 </sst>
 </file>
@@ -363,35 +363,35 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,7 +676,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,49 +692,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="A5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -747,7 +747,7 @@
     </row>
     <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -758,38 +758,38 @@
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="15"/>
+      <c r="E9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -799,13 +799,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>24</v>
@@ -813,54 +813,54 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A7:G7"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:G13"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>